<commit_message>
🔒 Security: Move API tokens to .env & cleanup repo
- Moved API_TOKEN and ADMIN_CHAT_ID to environment variables
- Created .env file (gitignored)
- Updated config.py to load from .env with validation
- Enhanced .gitignore with comprehensive patterns
- Removed unnecessary files (simulate_shark.py, bot_run.log)
- Deleted deprecated files (dnseGuide.txt, stock_lists.py)

Security improvements:
- No more hardcoded secrets in version control
- Added python-dotenv for env var management
- Proper error handling if env vars missing
</commit_message>
<xml_diff>
--- a/MaterialsDnse/DNSE - MDDS System - KRX v1.4.xlsx
+++ b/MaterialsDnse/DNSE - MDDS System - KRX v1.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/encap/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinhh/Documents/Bot/MaterialsDnse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C154B180-3BA3-9D45-BF05-6D538BF5ABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC50C2A-56DB-4D46-9C06-5128034C9864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="51200" windowHeight="27280" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -2846,7 +2846,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -3096,7 +3096,7 @@
   <dimension ref="A3:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A3" sqref="A3:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -3333,8 +3333,8 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4004,9 +4004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A3A105-54D8-9843-B0C3-FE0E64797400}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4145,7 +4145,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4317,7 +4317,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4397,7 +4397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>408</v>
       </c>
@@ -4425,8 +4425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC54DB3-CFF5-4F4B-BB82-3BB079C5B404}">
   <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView topLeftCell="A13" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:M149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7966,6 +7966,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7974,7 +7975,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>